<commit_message>
update to new version excel
</commit_message>
<xml_diff>
--- a/public/individual_jcic.xlsx
+++ b/public/individual_jcic.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="540" windowWidth="22400" windowHeight="10060"/>
@@ -11,9 +11,9 @@
     <sheet name="査証人名簿" sheetId="2" r:id="rId2"/>
     <sheet name="滞在予定表" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="130407"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>日本旅行社名</t>
   </si>
@@ -145,12 +145,6 @@
 電話：03-3470-6851</t>
   </si>
   <si>
-    <t>http://123.56.136.55/code</t>
-  </si>
-  <si>
-    <t>※编号请查询</t>
-  </si>
-  <si>
     <t>性别</t>
   </si>
   <si>
@@ -200,15 +194,65 @@
   <si>
     <t>个人</t>
   </si>
+  <si>
+    <t>访问城市</t>
+    <rPh sb="0" eb="2">
+      <t>faンg weン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>cheンg shi</t>
+    </rPh>
+    <phoneticPr fontId="21"/>
+  </si>
+  <si>
+    <t>沖縄県,宮城県</t>
+    <phoneticPr fontId="21"/>
+  </si>
+  <si>
+    <t>(沖縄県,青森県,岩手県,宮城県,秋田県,山形県,福島県)</t>
+    <rPh sb="1" eb="4">
+      <t>オキナワケン</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>アオモリケン</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>イワテケン</t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t>ミヤギケン</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>アキタケン</t>
+    </rPh>
+    <rPh sb="21" eb="24">
+      <t>ヤマガタケン</t>
+    </rPh>
+    <rPh sb="25" eb="28">
+      <t>フクシマケン</t>
+    </rPh>
+    <phoneticPr fontId="21"/>
+  </si>
+  <si>
+    <t>住宿城市</t>
+    <rPh sb="0" eb="2">
+      <t>zhu su</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>cheンg shi</t>
+    </rPh>
+    <phoneticPr fontId="21"/>
+  </si>
+  <si>
+    <t>沖縄県</t>
+    <phoneticPr fontId="21"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy/m/d"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -302,11 +346,6 @@
       <name val="宋体"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="55"/>
-      <name val="宋体"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color indexed="12"/>
@@ -337,6 +376,12 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -415,23 +460,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -459,43 +504,42 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -505,11 +549,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -526,13 +570,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
       <color rgb="FF969696"/>
@@ -572,7 +617,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -616,7 +661,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -665,7 +710,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -709,7 +754,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1018,19 +1063,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" customWidth="1"/>
@@ -1109,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1119,12 +1164,14 @@
     <row r="8" spans="1:7" ht="16.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="21" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
-      <c r="C8" s="25">
-        <v>43079</v>
+      <c r="C8" s="43" t="s">
+        <v>55</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1132,18 +1179,26 @@
     <row r="9" spans="1:7" ht="16.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="21" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
-      <c r="C9" s="25">
-        <v>43094</v>
+      <c r="C9" s="43" t="s">
+        <v>58</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="17.5" customHeight="1">
       <c r="A10" s="1"/>
+      <c r="B10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="25">
+        <v>43079</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1151,11 +1206,11 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="27" t="s">
-        <v>39</v>
+      <c r="B11" s="21" t="s">
+        <v>14</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>38</v>
+      <c r="C11" s="25">
+        <v>43094</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1218,11 +1273,11 @@
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="29" t="s">
-        <v>49</v>
+      <c r="C18" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1231,11 +1286,11 @@
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="29" t="s">
-        <v>40</v>
+      <c r="B19" s="28" t="s">
+        <v>38</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>41</v>
+      <c r="C19" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1244,11 +1299,11 @@
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="29" t="s">
-        <v>42</v>
+      <c r="B20" s="28" t="s">
+        <v>40</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>50</v>
+      <c r="C20" s="28" t="s">
+        <v>48</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1257,11 +1312,11 @@
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="29" t="s">
-        <v>43</v>
+      <c r="B21" s="28" t="s">
+        <v>41</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>44</v>
+      <c r="C21" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1270,11 +1325,11 @@
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="29" t="s">
-        <v>45</v>
+      <c r="B22" s="28" t="s">
+        <v>43</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>46</v>
+      <c r="C22" s="28" t="s">
+        <v>44</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1283,11 +1338,11 @@
     </row>
     <row r="23" spans="1:7" ht="28.25" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="31" t="s">
-        <v>47</v>
+      <c r="B23" s="30" t="s">
+        <v>45</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>52</v>
+      <c r="C23" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1296,11 +1351,11 @@
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1">
       <c r="A24" s="6"/>
-      <c r="B24" s="30" t="s">
-        <v>48</v>
+      <c r="B24" s="29" t="s">
+        <v>46</v>
       </c>
-      <c r="C24" s="30" t="s">
-        <v>51</v>
+      <c r="C24" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -8040,18 +8095,15 @@
       <c r="G986" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="22"/>
+  <phoneticPr fontId="21"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
       <formula1>"个人,冲绳东北六县多次,一定经济能力多次"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -8059,14 +8111,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
@@ -8080,52 +8132,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="str">
+      <c r="A3" s="37" t="e">
         <f>"（"&amp;YEAR(基本信息!C8)&amp;"年"&amp;MONTH(基本信息!C8)&amp;"月"&amp;DAY(基本信息!C8)&amp;"日 〜 "&amp;YEAR(基本信息!C9)&amp;"年"&amp;MONTH(基本信息!C9)&amp;"月"&amp;DAY(基本信息!C9)&amp;"日）"</f>
-        <v>（2017年12月10日 〜 2017年12月25日）</v>
+        <v>#VALUE!</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A4" s="38" t="str">
+      <c r="A4" s="37" t="str">
         <f>"（旅行参加者"&amp;MAX(A6:A15)&amp;"名、"&amp;"代表者"&amp;B6&amp;"、他"&amp;MAX(A6:A15)-1&amp;"名）"</f>
         <v>（旅行参加者1名、代表者王利、他0名）</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" ht="24" customHeight="1">
       <c r="A5" s="8" t="s">
@@ -8308,55 +8360,55 @@
       <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A17" s="35" t="str">
+      <c r="A17" s="34" t="str">
         <f>"公司名称："&amp;基本信息!C3</f>
         <v>公司名称：北京新日国際旅行社有限公司成都分公司</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A18" s="35" t="str">
+      <c r="A18" s="34" t="str">
         <f>"担当者："&amp;基本信息!C5</f>
         <v>担当者：小利</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
     </row>
     <row r="19" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A19" s="35" t="str">
+      <c r="A19" s="34" t="str">
         <f>"电话："&amp;基本信息!C6</f>
         <v>电话：0000-88983820</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
     </row>
     <row r="20" spans="1:8" ht="73.25" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" ht="14.25" customHeight="1">
       <c r="A21" s="7"/>
@@ -14219,11 +14271,11 @@
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <phoneticPr fontId="22"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -14231,14 +14283,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
@@ -14247,55 +14299,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="22.5" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1">
-      <c r="A2" s="43" t="str">
+      <c r="A2" s="42" t="e">
         <f>"（"&amp;YEAR(基本信息!C8)&amp;"年"&amp;MONTH(基本信息!C8)&amp;"月"&amp;DAY(基本信息!C8)&amp;"日 〜 "&amp;YEAR(基本信息!C9)&amp;"年"&amp;MONTH(基本信息!C9)&amp;"月"&amp;DAY(基本信息!C9)&amp;"日）"</f>
-        <v>（2017年12月10日 〜 2017年12月25日）</v>
+        <v>#VALUE!</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A3" s="40" t="str">
+      <c r="A3" s="39" t="str">
         <f>"（旅行参加者"&amp;MAX(査証人名簿!A6:A15)&amp;"名、"&amp;"代表者"&amp;査証人名簿!B6&amp;"、他"&amp;MAX(査証人名簿!A6:A15)-1&amp;"名）"</f>
         <v>（旅行参加者1名、代表者王利、他0名）</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:3" ht="25.5" customHeight="1">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="42" customHeight="1">
-      <c r="A5" s="16">
+      <c r="A5" s="16" t="str">
         <f>IF(AND(LEN(基本信息!C8),LEN(基本信息!C8)),基本信息!C8,"")</f>
-        <v>43079</v>
+        <v>沖縄県,宮城県</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="44.25" customHeight="1">
-      <c r="A6" s="16">
+      <c r="A6" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+1&lt;=基本信息!C9,A5+1,""),"")</f>
-        <v>43080</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>35</v>
@@ -14305,233 +14357,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="44.25" customHeight="1">
-      <c r="A7" s="16">
+      <c r="A7" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+2&lt;=基本信息!C9,A5+2,""),"")</f>
-        <v>43081</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
     </row>
     <row r="8" spans="1:3" ht="44.25" customHeight="1">
-      <c r="A8" s="16">
+      <c r="A8" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+3&lt;=基本信息!C9,A5+3,""),"")</f>
-        <v>43082</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:3" ht="42" customHeight="1">
-      <c r="A9" s="16">
+      <c r="A9" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+4&lt;=基本信息!C9,A5+4,""),"")</f>
-        <v>43083</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
     </row>
     <row r="10" spans="1:3" ht="42" customHeight="1">
-      <c r="A10" s="16">
+      <c r="A10" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+5&lt;=基本信息!C9,A5+5,""),"")</f>
-        <v>43084</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:3" ht="46.5" customHeight="1">
-      <c r="A11" s="16">
+      <c r="A11" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+6&lt;=基本信息!C9,A5+6,""),"")</f>
-        <v>43085</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:3" ht="47.25" customHeight="1">
-      <c r="A12" s="16">
+      <c r="A12" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+7&lt;=基本信息!C9,A5+7,""),"")</f>
-        <v>43086</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:3" ht="41.25" customHeight="1">
-      <c r="A13" s="16">
+      <c r="A13" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+8&lt;=基本信息!C9,A5+8,""),"")</f>
-        <v>43087</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:3" ht="42" customHeight="1">
-      <c r="A14" s="16">
+      <c r="A14" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+9&lt;=基本信息!C9,A5+9,""),"")</f>
-        <v>43088</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:3" ht="42" customHeight="1">
-      <c r="A15" s="16">
+      <c r="A15" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+10&lt;=基本信息!C9,A5+10,""),"")</f>
-        <v>43089</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A16" s="16">
+      <c r="A16" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+11&lt;=基本信息!C9,A5+11,""),"")</f>
-        <v>43090</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
     </row>
     <row r="17" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A17" s="16">
+      <c r="A17" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+12&lt;=基本信息!C9,A5+12,""),"")</f>
-        <v>43091</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
     </row>
     <row r="18" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A18" s="16">
+      <c r="A18" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+13&lt;=基本信息!C9,A5+13,""),"")</f>
-        <v>43092</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
     </row>
     <row r="19" spans="1:3" ht="40.5" customHeight="1">
-      <c r="A19" s="16">
+      <c r="A19" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+14&lt;=基本信息!C9,A5+14,""),"")</f>
-        <v>43093</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
     </row>
     <row r="20" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A20" s="16">
+      <c r="A20" s="16" t="e">
         <f>IF(LEN(A5),IF(A5+15&lt;=基本信息!C9,A5+15,""),"")</f>
-        <v>43094</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
     </row>
     <row r="21" spans="1:3" ht="41.25" customHeight="1">
-      <c r="A21" s="19" t="str">
+      <c r="A21" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+16&lt;=基本信息!C9,A5+16,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
     </row>
     <row r="22" spans="1:3" ht="40.5" customHeight="1">
-      <c r="A22" s="19" t="str">
+      <c r="A22" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+17&lt;=基本信息!C9,A5+17,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
     </row>
     <row r="23" spans="1:3" ht="39" customHeight="1">
-      <c r="A23" s="19" t="str">
+      <c r="A23" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+18&lt;=基本信息!C9,A5+18,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:3" ht="40.5" customHeight="1">
-      <c r="A24" s="19" t="str">
+      <c r="A24" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+19&lt;=基本信息!C9,A5+19,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
     </row>
     <row r="25" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A25" s="19" t="str">
+      <c r="A25" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+20&lt;=基本信息!C9,A5+20,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
     </row>
     <row r="26" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A26" s="19" t="str">
+      <c r="A26" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+21&lt;=基本信息!C9,A5+21,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:3" ht="39" customHeight="1">
-      <c r="A27" s="19" t="str">
+      <c r="A27" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+22&lt;=基本信息!C9,A5+22,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
     </row>
     <row r="28" spans="1:3" ht="39" customHeight="1">
-      <c r="A28" s="19" t="str">
+      <c r="A28" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+23&lt;=基本信息!C9,A5+23,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
     </row>
     <row r="29" spans="1:3" ht="39" customHeight="1">
-      <c r="A29" s="19" t="str">
+      <c r="A29" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+24&lt;=基本信息!C9,A5+24,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
     </row>
     <row r="30" spans="1:3" ht="38.25" customHeight="1">
-      <c r="A30" s="19" t="str">
+      <c r="A30" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+25&lt;=基本信息!C9,A5+25,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
     </row>
     <row r="31" spans="1:3" ht="39" customHeight="1">
-      <c r="A31" s="19" t="str">
+      <c r="A31" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+26&lt;=基本信息!C9,A5+26,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
     </row>
     <row r="32" spans="1:3" ht="38.25" customHeight="1">
-      <c r="A32" s="19" t="str">
+      <c r="A32" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+27&lt;=基本信息!C9,A5+27,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
     </row>
     <row r="33" spans="1:3" ht="37.5" customHeight="1">
-      <c r="A33" s="19" t="str">
+      <c r="A33" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+28&lt;=基本信息!C9,A5+28,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
     </row>
     <row r="34" spans="1:3" ht="39.5" customHeight="1">
-      <c r="A34" s="19" t="str">
+      <c r="A34" s="19" t="e">
         <f>IF(LEN(A5),IF(A5+29&lt;=基本信息!C9,A5+29,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
     </row>
     <row r="35" spans="1:3" ht="40.75" customHeight="1">
-      <c r="A35" s="20" t="str">
+      <c r="A35" s="20" t="e">
         <f>IF(LEN(A5),IF(A5+30&lt;=基本信息!C9,A5+30,""),"")</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -14542,33 +14594,33 @@
       <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" s="42" t="str">
+      <c r="A37" s="41" t="str">
         <f>"公司名称："&amp;基本信息!C3</f>
         <v>公司名称：北京新日国際旅行社有限公司成都分公司</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" s="42" t="str">
+      <c r="A38" s="41" t="str">
         <f>"担当者："&amp;基本信息!C5</f>
         <v>担当者：小利</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" s="42" t="str">
+      <c r="A39" s="41" t="str">
         <f>"电话："&amp;基本信息!C6</f>
         <v>电话：0000-88983820</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
     </row>
     <row r="40" spans="1:3" ht="83.5" customHeight="1">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>37</v>
       </c>
     </row>
@@ -19395,11 +19447,11 @@
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A2:C2"/>
   </mergeCells>
-  <phoneticPr fontId="22"/>
+  <phoneticPr fontId="21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
fix xlsx bug again
</commit_message>
<xml_diff>
--- a/public/individual_jcic.xlsx
+++ b/public/individual_jcic.xlsx
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:G986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -14287,7 +14287,7 @@
   <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -14333,9 +14333,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="42" customHeight="1">
-      <c r="A5" s="16" t="str">
-        <f>IF(AND(LEN(基本信息!C8),LEN(基本信息!C8)),基本信息!C8,"")</f>
-        <v>沖縄県,宮城県</v>
+      <c r="A5" s="16">
+        <v>43079</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>52</v>
@@ -14345,9 +14344,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="44.25" customHeight="1">
-      <c r="A6" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+1&lt;=基本信息!C9,A5+1,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A6" s="16">
+        <v>43080</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>35</v>
@@ -14357,234 +14355,175 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="44.25" customHeight="1">
-      <c r="A7" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+2&lt;=基本信息!C9,A5+2,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A7" s="16">
+        <v>43081</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
     </row>
     <row r="8" spans="1:3" ht="44.25" customHeight="1">
-      <c r="A8" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+3&lt;=基本信息!C9,A5+3,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A8" s="16">
+        <v>43082</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:3" ht="42" customHeight="1">
-      <c r="A9" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+4&lt;=基本信息!C9,A5+4,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A9" s="16">
+        <v>43083</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
     </row>
     <row r="10" spans="1:3" ht="42" customHeight="1">
-      <c r="A10" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+5&lt;=基本信息!C9,A5+5,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A10" s="16">
+        <v>43084</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:3" ht="46.5" customHeight="1">
-      <c r="A11" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+6&lt;=基本信息!C9,A5+6,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A11" s="16">
+        <v>43085</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:3" ht="47.25" customHeight="1">
-      <c r="A12" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+7&lt;=基本信息!C9,A5+7,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A12" s="16">
+        <v>43086</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:3" ht="41.25" customHeight="1">
-      <c r="A13" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+8&lt;=基本信息!C9,A5+8,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A13" s="16">
+        <v>43087</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:3" ht="42" customHeight="1">
-      <c r="A14" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+9&lt;=基本信息!C9,A5+9,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A14" s="16">
+        <v>43088</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:3" ht="42" customHeight="1">
-      <c r="A15" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+10&lt;=基本信息!C9,A5+10,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A15" s="16">
+        <v>43089</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A16" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+11&lt;=基本信息!C9,A5+11,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A16" s="16">
+        <v>43090</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
     </row>
     <row r="17" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A17" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+12&lt;=基本信息!C9,A5+12,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A17" s="16">
+        <v>43091</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
     </row>
     <row r="18" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A18" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+13&lt;=基本信息!C9,A5+13,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A18" s="16">
+        <v>43092</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
     </row>
     <row r="19" spans="1:3" ht="40.5" customHeight="1">
-      <c r="A19" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+14&lt;=基本信息!C9,A5+14,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A19" s="16">
+        <v>43093</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
     </row>
     <row r="20" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A20" s="16" t="e">
-        <f>IF(LEN(A5),IF(A5+15&lt;=基本信息!C9,A5+15,""),"")</f>
-        <v>#VALUE!</v>
+      <c r="A20" s="16">
+        <v>43094</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
     </row>
     <row r="21" spans="1:3" ht="41.25" customHeight="1">
-      <c r="A21" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+16&lt;=基本信息!C9,A5+16,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A21" s="19"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
     </row>
     <row r="22" spans="1:3" ht="40.5" customHeight="1">
-      <c r="A22" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+17&lt;=基本信息!C9,A5+17,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A22" s="19"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
     </row>
     <row r="23" spans="1:3" ht="39" customHeight="1">
-      <c r="A23" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+18&lt;=基本信息!C9,A5+18,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A23" s="19"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:3" ht="40.5" customHeight="1">
-      <c r="A24" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+19&lt;=基本信息!C9,A5+19,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A24" s="19"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
     </row>
     <row r="25" spans="1:3" ht="39.75" customHeight="1">
-      <c r="A25" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+20&lt;=基本信息!C9,A5+20,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A25" s="19"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
     </row>
     <row r="26" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A26" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+21&lt;=基本信息!C9,A5+21,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A26" s="19"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:3" ht="39" customHeight="1">
-      <c r="A27" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+22&lt;=基本信息!C9,A5+22,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A27" s="19"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
     </row>
     <row r="28" spans="1:3" ht="39" customHeight="1">
-      <c r="A28" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+23&lt;=基本信息!C9,A5+23,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A28" s="19"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
     </row>
     <row r="29" spans="1:3" ht="39" customHeight="1">
-      <c r="A29" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+24&lt;=基本信息!C9,A5+24,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A29" s="19"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
     </row>
     <row r="30" spans="1:3" ht="38.25" customHeight="1">
-      <c r="A30" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+25&lt;=基本信息!C9,A5+25,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A30" s="19"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
     </row>
     <row r="31" spans="1:3" ht="39" customHeight="1">
-      <c r="A31" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+26&lt;=基本信息!C9,A5+26,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A31" s="19"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
     </row>
     <row r="32" spans="1:3" ht="38.25" customHeight="1">
-      <c r="A32" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+27&lt;=基本信息!C9,A5+27,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A32" s="19"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
     </row>
     <row r="33" spans="1:3" ht="37.5" customHeight="1">
-      <c r="A33" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+28&lt;=基本信息!C9,A5+28,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A33" s="19"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
     </row>
     <row r="34" spans="1:3" ht="39.5" customHeight="1">
-      <c r="A34" s="19" t="e">
-        <f>IF(LEN(A5),IF(A5+29&lt;=基本信息!C9,A5+29,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A34" s="19"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
     </row>
     <row r="35" spans="1:3" ht="40.75" customHeight="1">
-      <c r="A35" s="20" t="e">
-        <f>IF(LEN(A5),IF(A5+30&lt;=基本信息!C9,A5+30,""),"")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A35" s="20"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
     </row>

</xml_diff>